<commit_message>
Fix an issue loading custom formats
</commit_message>
<xml_diff>
--- a/test_xlsx_data/test_file_2.xlsx
+++ b/test_xlsx_data/test_file_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16620" activeTab="2"/>
+    <workbookView windowHeight="16560"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -112,7 +112,7 @@
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="[$-809]dd\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -717,10 +717,9 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="18" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -995,15 +994,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="7"/>
   <cols>
-    <col min="3" max="3" width="15.25"/>
+    <col min="3" max="3" width="15.25" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1013,7 +1012,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -1054,22 +1053,22 @@
       <c r="E2">
         <v>20</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>0.12</v>
       </c>
-      <c r="G2" s="5" t="str">
+      <c r="G2" s="4" t="str">
         <f>IFERROR(VLOOKUP(A2,Countries!$A$1:$B$4,2,FALSE),"?")</f>
         <v>Belgium</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="4">
         <f t="shared" ref="H2:H8" si="0">D2*E2</f>
         <v>200</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="4">
         <f t="shared" ref="I2:I8" si="1">H2*F2</f>
         <v>24</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="4">
         <f t="shared" ref="J2:J8" si="2">H2+I2</f>
         <v>224</v>
       </c>
@@ -1090,22 +1089,22 @@
       <c r="E3">
         <v>17</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>0.12</v>
       </c>
-      <c r="G3" s="5" t="str">
+      <c r="G3" s="4" t="str">
         <f>IFERROR(VLOOKUP(A3,Countries!$A$1:$B$4,2,FALSE),"?")</f>
         <v>Belgium</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="4">
         <f t="shared" si="0"/>
         <v>102</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="4">
         <f t="shared" si="1"/>
         <v>12.24</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="4">
         <f t="shared" si="2"/>
         <v>114.24</v>
       </c>
@@ -1126,22 +1125,22 @@
       <c r="E4">
         <v>36</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>0.05</v>
       </c>
-      <c r="G4" s="5" t="str">
+      <c r="G4" s="4" t="str">
         <f>IFERROR(VLOOKUP(A4,Countries!$A$1:$B$4,2,FALSE),"?")</f>
         <v>Belgium</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="4">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <f t="shared" si="1"/>
         <v>3.6</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="4">
         <f t="shared" si="2"/>
         <v>75.6</v>
       </c>
@@ -1162,22 +1161,22 @@
       <c r="E5">
         <v>100</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>0.12</v>
       </c>
-      <c r="G5" s="5" t="str">
+      <c r="G5" s="4" t="str">
         <f>IFERROR(VLOOKUP(A5,Countries!$A$1:$B$4,2,FALSE),"?")</f>
         <v>Belgium</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="4">
         <f t="shared" si="2"/>
         <v>112</v>
       </c>
@@ -1198,22 +1197,22 @@
       <c r="E6">
         <v>20</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>0.07</v>
       </c>
-      <c r="G6" s="5" t="str">
+      <c r="G6" s="4" t="str">
         <f>IFERROR(VLOOKUP(A6,Countries!$A$1:$B$4,2,FALSE),"?")</f>
         <v>France</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <f t="shared" si="1"/>
         <v>4.2</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="4">
         <f t="shared" si="2"/>
         <v>64.2</v>
       </c>
@@ -1234,22 +1233,22 @@
       <c r="E7">
         <v>17</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>0.07</v>
       </c>
-      <c r="G7" s="5" t="str">
+      <c r="G7" s="4" t="str">
         <f>IFERROR(VLOOKUP(A7,Countries!$A$1:$B$4,2,FALSE),"?")</f>
         <v>France</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <f t="shared" si="0"/>
         <v>102</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="4">
         <f t="shared" si="1"/>
         <v>7.14</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="4">
         <f t="shared" si="2"/>
         <v>109.14</v>
       </c>
@@ -1270,28 +1269,25 @@
       <c r="E8">
         <v>36</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>0.08</v>
       </c>
-      <c r="G8" s="5" t="str">
+      <c r="G8" s="4" t="str">
         <f>IFERROR(VLOOKUP(A8,Countries!$A$1:$B$4,2,FALSE),"?")</f>
         <v>?</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="4">
         <f t="shared" si="0"/>
         <v>324</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="4">
         <f t="shared" si="1"/>
         <v>25.92</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="4">
         <f t="shared" si="2"/>
         <v>349.92</v>
       </c>
-    </row>
-    <row r="17" spans="3:3">
-      <c r="C17" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1424,7 +1420,7 @@
   <sheetPr/>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add support to load definition of named ranges. Refactor loadWorkbook. Migrate Xojo version
</commit_message>
<xml_diff>
--- a/test_xlsx_data/test_file_2.xlsx
+++ b/test_xlsx_data/test_file_2.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17680"/>
+    <workbookView windowHeight="16020"/>
   </bookViews>
   <sheets>
-    <sheet name="Sales data" sheetId="1" r:id="rId1"/>
-    <sheet name="Countries" sheetId="3" r:id="rId2"/>
-    <sheet name="Summary" sheetId="2" r:id="rId3"/>
+    <sheet name="Sales data 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sales data 2" sheetId="5" r:id="rId2"/>
+    <sheet name="Countries" sheetId="3" r:id="rId3"/>
+    <sheet name="Summary" sheetId="2" r:id="rId4"/>
+    <sheet name="Parameters" sheetId="4" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="Block2">Parameters!$B$12:$D$16</definedName>
+    <definedName name="AlphaBlock">Parameters!$B$3:$D$7</definedName>
+    <definedName name="SalesCountry" localSheetId="0">'Sales data 1'!$G$1:$G$8</definedName>
+    <definedName name="SalesCountry" localSheetId="1">'Sales data 2'!$G$1:$G$8</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -29,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="37">
   <si>
     <t>City</t>
   </si>
@@ -101,6 +109,45 @@
   </si>
   <si>
     <t>% Of total</t>
+  </si>
+  <si>
+    <t>Param_Bloc1</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>bbb</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>cccc</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>ddddd</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>Param_Block2</t>
+  </si>
+  <si>
+    <t>Alpha2</t>
+  </si>
+  <si>
+    <t>Beta2</t>
+  </si>
+  <si>
+    <t>Gamma2</t>
   </si>
 </sst>
 </file>
@@ -996,7 +1043,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="G1" sqref="G1:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="7"/>
@@ -1055,9 +1102,8 @@
       <c r="F2" s="6">
         <v>0.12</v>
       </c>
-      <c r="G2" s="7" t="str">
-        <f>IFERROR(VLOOKUP(A2,Countries!$A$1:$B$4,2,FALSE),"?")</f>
-        <v>Belgium</v>
+      <c r="G2" t="s">
+        <v>6</v>
       </c>
       <c r="H2" s="7">
         <f t="shared" ref="H2:H8" si="0">D2*E2</f>
@@ -1091,9 +1137,8 @@
       <c r="F3" s="6">
         <v>0.12</v>
       </c>
-      <c r="G3" s="7" t="str">
-        <f>IFERROR(VLOOKUP(A3,Countries!$A$1:$B$4,2,FALSE),"?")</f>
-        <v>Belgium</v>
+      <c r="G3" t="s">
+        <v>6</v>
       </c>
       <c r="H3" s="7">
         <f t="shared" si="0"/>
@@ -1127,9 +1172,8 @@
       <c r="F4" s="6">
         <v>0.05</v>
       </c>
-      <c r="G4" s="7" t="str">
-        <f>IFERROR(VLOOKUP(A4,Countries!$A$1:$B$4,2,FALSE),"?")</f>
-        <v>Belgium</v>
+      <c r="G4" t="s">
+        <v>6</v>
       </c>
       <c r="H4" s="7">
         <f t="shared" si="0"/>
@@ -1163,9 +1207,8 @@
       <c r="F5" s="6">
         <v>0.12</v>
       </c>
-      <c r="G5" s="7" t="str">
-        <f>IFERROR(VLOOKUP(A5,Countries!$A$1:$B$4,2,FALSE),"?")</f>
-        <v>Belgium</v>
+      <c r="G5" t="s">
+        <v>6</v>
       </c>
       <c r="H5" s="7">
         <f t="shared" si="0"/>
@@ -1199,9 +1242,8 @@
       <c r="F6" s="6">
         <v>0.07</v>
       </c>
-      <c r="G6" s="7" t="str">
-        <f>IFERROR(VLOOKUP(A6,Countries!$A$1:$B$4,2,FALSE),"?")</f>
-        <v>France</v>
+      <c r="G6" t="s">
+        <v>6</v>
       </c>
       <c r="H6" s="7">
         <f t="shared" si="0"/>
@@ -1235,9 +1277,8 @@
       <c r="F7" s="6">
         <v>0.07</v>
       </c>
-      <c r="G7" s="7" t="str">
-        <f>IFERROR(VLOOKUP(A7,Countries!$A$1:$B$4,2,FALSE),"?")</f>
-        <v>France</v>
+      <c r="G7" t="s">
+        <v>6</v>
       </c>
       <c r="H7" s="7">
         <f t="shared" si="0"/>
@@ -1271,9 +1312,8 @@
       <c r="F8" s="6">
         <v>0.08</v>
       </c>
-      <c r="G8" s="7" t="str">
-        <f>IFERROR(VLOOKUP(A8,Countries!$A$1:$B$4,2,FALSE),"?")</f>
-        <v>?</v>
+      <c r="G8" t="s">
+        <v>6</v>
       </c>
       <c r="H8" s="7">
         <f t="shared" si="0"/>
@@ -1296,6 +1336,311 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="7"/>
+  <cols>
+    <col min="3" max="3" width="30.421875" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2">
+        <v>45577</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="G2" s="7" t="str">
+        <f>IFERROR(VLOOKUP(A2,Countries!$A$1:$B$4,2,FALSE),"?")</f>
+        <v>Belgium</v>
+      </c>
+      <c r="H2" s="7">
+        <f t="shared" ref="H2:H8" si="0">D2*E2</f>
+        <v>200</v>
+      </c>
+      <c r="I2" s="7">
+        <f t="shared" ref="I2:I8" si="1">H2*F2</f>
+        <v>24</v>
+      </c>
+      <c r="J2" s="7">
+        <f t="shared" ref="J2:J8" si="2">H2+I2</f>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2">
+        <v>45577</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>17</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="G3" s="7" t="str">
+        <f>IFERROR(VLOOKUP(A3,Countries!$A$1:$B$4,2,FALSE),"?")</f>
+        <v>Belgium</v>
+      </c>
+      <c r="H3" s="7">
+        <f t="shared" si="0"/>
+        <v>102</v>
+      </c>
+      <c r="I3" s="7">
+        <f t="shared" si="1"/>
+        <v>12.24</v>
+      </c>
+      <c r="J3" s="7">
+        <f t="shared" si="2"/>
+        <v>114.24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2">
+        <v>45637</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>36</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="G4" s="7" t="str">
+        <f>IFERROR(VLOOKUP(A4,Countries!$A$1:$B$4,2,FALSE),"?")</f>
+        <v>Belgium</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="1"/>
+        <v>3.6</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="2"/>
+        <v>75.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3">
+        <v>45640</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="G5" s="7" t="str">
+        <f>IFERROR(VLOOKUP(A5,Countries!$A$1:$B$4,2,FALSE),"?")</f>
+        <v>Belgium</v>
+      </c>
+      <c r="H5" s="7">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="I5" s="7">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="J5" s="7">
+        <f t="shared" si="2"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="4">
+        <v>45577</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0.07</v>
+      </c>
+      <c r="G6" s="7" t="str">
+        <f>IFERROR(VLOOKUP(A6,Countries!$A$1:$B$4,2,FALSE),"?")</f>
+        <v>France</v>
+      </c>
+      <c r="H6" s="7">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="I6" s="7">
+        <f t="shared" si="1"/>
+        <v>4.2</v>
+      </c>
+      <c r="J6" s="7">
+        <f t="shared" si="2"/>
+        <v>64.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="5">
+        <v>45637</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>17</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0.07</v>
+      </c>
+      <c r="G7" s="7" t="str">
+        <f>IFERROR(VLOOKUP(A7,Countries!$A$1:$B$4,2,FALSE),"?")</f>
+        <v>France</v>
+      </c>
+      <c r="H7" s="7">
+        <f t="shared" si="0"/>
+        <v>102</v>
+      </c>
+      <c r="I7" s="7">
+        <f t="shared" si="1"/>
+        <v>7.14</v>
+      </c>
+      <c r="J7" s="7">
+        <f t="shared" si="2"/>
+        <v>109.14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="5">
+        <v>45640</v>
+      </c>
+      <c r="D8">
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <v>36</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0.08</v>
+      </c>
+      <c r="G8" s="7" t="str">
+        <f>IFERROR(VLOOKUP(A8,Countries!$A$1:$B$4,2,FALSE),"?")</f>
+        <v>?</v>
+      </c>
+      <c r="H8" s="7">
+        <f t="shared" si="0"/>
+        <v>324</v>
+      </c>
+      <c r="I8" s="7">
+        <f t="shared" si="1"/>
+        <v>25.92</v>
+      </c>
+      <c r="J8" s="7">
+        <f t="shared" si="2"/>
+        <v>349.92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="600" verticalDpi="600"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:B4"/>
@@ -1345,13 +1690,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="4" outlineLevelCol="4"/>
@@ -1378,15 +1723,15 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <f>SUMIFS('Sales data'!H:H,'Sales data'!$A:$A,$A2)</f>
+        <f>SUMIFS('Sales data 1'!H:H,'Sales data 1'!$A:$A,$A2)</f>
         <v>72</v>
       </c>
       <c r="C2">
-        <f>SUMIFS('Sales data'!I:I,'Sales data'!$A:$A,$A2)</f>
+        <f>SUMIFS('Sales data 1'!I:I,'Sales data 1'!$A:$A,$A2)</f>
         <v>3.6</v>
       </c>
       <c r="D2">
-        <f>SUMIFS('Sales data'!J:J,'Sales data'!$A:$A,$A2)</f>
+        <f>SUMIFS('Sales data 1'!J:J,'Sales data 1'!$A:$A,$A2)</f>
         <v>75.6</v>
       </c>
       <c r="E2" s="1">
@@ -1399,15 +1744,15 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <f>SUMIFS('Sales data'!H:H,'Sales data'!$A:$A,$A3)</f>
+        <f>SUMIFS('Sales data 1'!H:H,'Sales data 1'!$A:$A,$A3)</f>
         <v>402</v>
       </c>
       <c r="C3">
-        <f>SUMIFS('Sales data'!I:I,'Sales data'!$A:$A,$A3)</f>
+        <f>SUMIFS('Sales data 1'!I:I,'Sales data 1'!$A:$A,$A3)</f>
         <v>48.24</v>
       </c>
       <c r="D3">
-        <f>SUMIFS('Sales data'!J:J,'Sales data'!$A:$A,$A3)</f>
+        <f>SUMIFS('Sales data 1'!J:J,'Sales data 1'!$A:$A,$A3)</f>
         <v>450.24</v>
       </c>
       <c r="E3" s="1">
@@ -1420,15 +1765,15 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <f>SUMIFS('Sales data'!H:H,'Sales data'!$A:$A,$A4)</f>
+        <f>SUMIFS('Sales data 1'!H:H,'Sales data 1'!$A:$A,$A4)</f>
         <v>162</v>
       </c>
       <c r="C4">
-        <f>SUMIFS('Sales data'!I:I,'Sales data'!$A:$A,$A4)</f>
+        <f>SUMIFS('Sales data 1'!I:I,'Sales data 1'!$A:$A,$A4)</f>
         <v>11.34</v>
       </c>
       <c r="D4">
-        <f>SUMIFS('Sales data'!J:J,'Sales data'!$A:$A,$A4)</f>
+        <f>SUMIFS('Sales data 1'!J:J,'Sales data 1'!$A:$A,$A4)</f>
         <v>173.34</v>
       </c>
       <c r="E4" s="1">
@@ -1441,15 +1786,15 @@
         <v>18</v>
       </c>
       <c r="B5">
-        <f>SUMIFS('Sales data'!H:H,'Sales data'!$A:$A,$A5)</f>
+        <f>SUMIFS('Sales data 1'!H:H,'Sales data 1'!$A:$A,$A5)</f>
         <v>324</v>
       </c>
       <c r="C5">
-        <f>SUMIFS('Sales data'!I:I,'Sales data'!$A:$A,$A5)</f>
+        <f>SUMIFS('Sales data 1'!I:I,'Sales data 1'!$A:$A,$A5)</f>
         <v>25.92</v>
       </c>
       <c r="D5">
-        <f>SUMIFS('Sales data'!J:J,'Sales data'!$A:$A,$A5)</f>
+        <f>SUMIFS('Sales data 1'!J:J,'Sales data 1'!$A:$A,$A5)</f>
         <v>349.92</v>
       </c>
       <c r="E5" s="1">
@@ -1462,4 +1807,144 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="600" verticalDpi="600"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="B2:D16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="3"/>
+  <sheetData>
+    <row r="2" spans="2:2">
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16">
+        <v>444</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="B4:D7">
+    <sortCondition ref="B4"/>
+  </sortState>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>